<commit_message>
Actualizacion para Excel 2010
Librerías para excel 2010 y cambio de leyenda institucional a "2022 - LAS MALVINAS SON ARGENTINAS"
</commit_message>
<xml_diff>
--- a/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
+++ b/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="156" windowWidth="20052" windowHeight="7932"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -85,14 +85,14 @@
     <t>MaxHold manual c/incert V/m</t>
   </si>
   <si>
-    <t>2020 - AÑO DEL GENERAL MANUEL BELGRANO</t>
+    <t>2022 - LAS MALVINAS SON ARGENTINAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,11 +215,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -227,6 +227,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -348,6 +353,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -382,6 +388,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -557,60 +564,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="M6" sqref="L6:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="5.85546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="11" max="11" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.88671875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="5.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.75">
-      <c r="P1" s="9" t="s">
+    <row r="1" spans="1:16" ht="13.8" x14ac:dyDescent="0.2">
+      <c r="P1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="18.75">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="12" thickBot="1"/>
-    <row r="9" spans="1:16" s="2" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:16" s="2" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -660,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -674,7 +681,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -688,7 +695,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -702,7 +709,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -716,7 +723,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -730,7 +737,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -744,7 +751,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -758,7 +765,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -789,26 +796,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
v1.13.10 - Nuevo logo ENACOM 2022
Se actualizaron logos, iconos y leyenda institucional de ENACOM 2022
</commit_message>
<xml_diff>
--- a/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
+++ b/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
@@ -85,7 +85,7 @@
     <t>MaxHold manual c/incert V/m</t>
   </si>
   <si>
-    <t>2022 - LAS MALVINAS SON ARGENTINAS</t>
+    <t>2022 - Las Malvinas son argentinas</t>
   </si>
 </sst>
 </file>
@@ -240,33 +240,39 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>7619</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>10128</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>125048</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>798315</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="3 Imagen" descr="ENACOM_contexto_final.jpg"/>
+        <xdr:cNvPr id="4" name="3 Imagen"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1"/>
-          <a:ext cx="1229948" cy="847724"/>
+          <a:off x="7619" y="10128"/>
+          <a:ext cx="2459476" cy="538512"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -569,7 +575,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="L6:M6"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change error msg on startup and remove xlsx legend
- Se removieron las leyendas institucionales de los reportes XLSX para que no deban modificarse cada año
- Se modificó un mensaje de error al no encontrar archivos de incertidumbre en el startup
</commit_message>
<xml_diff>
--- a/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
+++ b/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="156" windowWidth="20052" windowHeight="7932"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Indice</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>MaxHold manual c/incert V/m</t>
-  </si>
-  <si>
-    <t>2022 - Las Malvinas son argentinas</t>
   </si>
 </sst>
 </file>
@@ -575,32 +572,30 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.44140625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="5.88671875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.44140625" style="1"/>
+    <col min="11" max="11" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="5.85546875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="P1" s="8" t="s">
-        <v>17</v>
-      </c>
+    <row r="1" spans="1:16" ht="13.9" x14ac:dyDescent="0.2">
+      <c r="P1" s="8"/>
     </row>
     <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
@@ -622,7 +617,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="10.9" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:16" s="2" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>0</v>
@@ -673,7 +668,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -687,7 +682,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -701,7 +696,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -715,7 +710,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -729,7 +724,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -743,7 +738,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -757,7 +752,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -771,7 +766,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="10.15" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -808,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -821,7 +816,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
v2.0.5 - Fix NMEA GPS zero minutes issue
- Se soluciona el problema del cambio de grados que corrompía datos y medición: se implementó clase NMEA0183Reader para interfaz exclusiva con GPS que funcionen bajo COM virtual y entreguen datos NMEA (separación de responsabilidades).
- Se actualizó logo institucional en los reportes de Excel.
</commit_message>
<xml_diff>
--- a/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
+++ b/Rastreador GPS+Maps/Resources/Modelo_averif.xlsx
@@ -237,13 +237,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7619</xdr:colOff>
+      <xdr:colOff>263519</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>10128</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>798315</xdr:colOff>
+      <xdr:colOff>542415</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -255,7 +255,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -268,8 +268,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7619" y="10128"/>
-          <a:ext cx="2459476" cy="538512"/>
+          <a:off x="263519" y="10128"/>
+          <a:ext cx="1945771" cy="561372"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>